<commit_message>
Attempt to resolve large file issue
</commit_message>
<xml_diff>
--- a/seasons/AmericanFootball/NationalFootballLeague/2023/forecasts/matrix_CON.xlsx
+++ b/seasons/AmericanFootball/NationalFootballLeague/2023/forecasts/matrix_CON.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SportPredictifier\SportPredictifier\seasons\AmericanFootball\NationalFootballLeague\2023\forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BA9DC0E0-765B-456E-B99E-454744AC295C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C882F9-5FC3-447E-8BAD-44309373BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected Bracket" sheetId="2" r:id="rId1"/>
     <sheet name="matrix_CON" sheetId="1" r:id="rId2"/>
     <sheet name="Forecasts" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>BAL</t>
   </si>
@@ -160,12 +195,18 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>SB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#0"/>
     <numFmt numFmtId="165" formatCode="#0%"/>
@@ -1007,7 +1048,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1050,8 +1091,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1071,31 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1206,29 +1224,54 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1268,6 +1311,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1601,10 +1645,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
@@ -1660,10 +1704,10 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="51"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -1672,7 +1716,7 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
-      <c r="U3" s="9"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
@@ -1684,10 +1728,10 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="11"/>
+      <c r="L4" s="53"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -1696,7 +1740,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
-      <c r="U4" s="9"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
@@ -1708,10 +1752,10 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="13"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -1720,7 +1764,7 @@
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
-      <c r="U5" s="9"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
@@ -1732,10 +1776,10 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="57"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1744,7 +1788,7 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
-      <c r="U6" s="9"/>
+      <c r="U6" s="7"/>
     </row>
     <row r="7" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
@@ -1756,7 +1800,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="16"/>
+      <c r="K7" s="8"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -1766,7 +1810,7 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
-      <c r="U7" s="9"/>
+      <c r="U7" s="7"/>
     </row>
     <row r="8" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
@@ -1777,14 +1821,14 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -1792,7 +1836,7 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-      <c r="U8" s="9"/>
+      <c r="U8" s="7"/>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
@@ -1802,15 +1846,15 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="21">
+      <c r="K9" s="13">
         <v>24.156864800000001</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="14">
         <v>22.389658600000001</v>
       </c>
-      <c r="M9" s="20"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1818,7 +1862,7 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
-      <c r="U9" s="9"/>
+      <c r="U9" s="7"/>
     </row>
     <row r="10" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
@@ -1828,11 +1872,11 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="20"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="20"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1840,7 +1884,7 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
-      <c r="U10" s="9"/>
+      <c r="U10" s="7"/>
     </row>
     <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
@@ -1850,18 +1894,18 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="49" t="s">
         <v>1</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="17" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="6"/>
@@ -1870,7 +1914,7 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
-      <c r="U11" s="9"/>
+      <c r="U11" s="7"/>
     </row>
     <row r="12" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
@@ -1880,18 +1924,18 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="57">
+      <c r="I12" s="48">
         <v>23.1765534</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="14">
         <v>16.541399800000001</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="21">
+      <c r="M12" s="13">
         <v>29.815231199999999</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="14">
         <v>22.66187</v>
       </c>
       <c r="O12" s="6"/>
@@ -1900,7 +1944,7 @@
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
-      <c r="U12" s="9"/>
+      <c r="U12" s="7"/>
     </row>
     <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
@@ -1910,11 +1954,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="20"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="20"/>
+      <c r="M13" s="12"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -1922,219 +1966,219 @@
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
-      <c r="U13" s="9"/>
+      <c r="U13" s="7"/>
     </row>
     <row r="14" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="26" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="23" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="20" t="s">
         <v>9</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="30" t="s">
+      <c r="N14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="31" t="s">
+      <c r="O14" s="9"/>
+      <c r="P14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="Q14" s="32" t="s">
+      <c r="Q14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="6"/>
-      <c r="U14" s="9"/>
+      <c r="U14" s="7"/>
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
-      <c r="C15" s="20"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="44">
+      <c r="F15" s="36">
         <v>24</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="37">
         <v>27</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="42">
+      <c r="I15" s="34">
         <v>34</v>
       </c>
-      <c r="J15" s="43">
+      <c r="J15" s="35">
         <v>10</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="42">
+      <c r="M15" s="34">
         <v>24</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="35">
         <v>21</v>
       </c>
       <c r="O15" s="6"/>
-      <c r="P15" s="42">
+      <c r="P15" s="34">
         <v>31</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="35">
         <v>23</v>
       </c>
       <c r="R15" s="6"/>
-      <c r="S15" s="20"/>
+      <c r="S15" s="12"/>
       <c r="T15" s="6"/>
-      <c r="U15" s="9"/>
+      <c r="U15" s="7"/>
     </row>
     <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
-      <c r="C16" s="20"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="20"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="20"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="20"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="20"/>
+      <c r="S16" s="12"/>
       <c r="T16" s="6"/>
-      <c r="U16" s="9"/>
+      <c r="U16" s="7"/>
     </row>
     <row r="17" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="27" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="29" t="s">
         <v>14</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="38" t="s">
+      <c r="M17" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="22" t="s">
         <v>10</v>
       </c>
       <c r="O17" s="6"/>
-      <c r="P17" s="31" t="s">
+      <c r="P17" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="39" t="s">
+      <c r="Q17" s="31" t="s">
         <v>16</v>
       </c>
       <c r="R17" s="6"/>
-      <c r="S17" s="40" t="s">
+      <c r="S17" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="T17" s="41" t="s">
+      <c r="T17" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="U17" s="9"/>
+      <c r="U17" s="7"/>
     </row>
     <row r="18" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="42">
+      <c r="C18" s="34">
         <v>31</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="35">
         <v>17</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="42">
+      <c r="F18" s="34">
         <v>26</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="35">
         <v>7</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="42">
+      <c r="I18" s="34">
         <v>45</v>
       </c>
-      <c r="J18" s="43">
+      <c r="J18" s="35">
         <v>14</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="44">
+      <c r="M18" s="36">
         <v>32</v>
       </c>
-      <c r="N18" s="45">
+      <c r="N18" s="37">
         <v>48</v>
       </c>
       <c r="O18" s="6"/>
-      <c r="P18" s="42">
+      <c r="P18" s="34">
         <v>24</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="Q18" s="35">
         <v>23</v>
       </c>
       <c r="R18" s="6"/>
-      <c r="S18" s="42">
+      <c r="S18" s="34">
         <v>32</v>
       </c>
-      <c r="T18" s="43">
+      <c r="T18" s="35">
         <v>9</v>
       </c>
-      <c r="U18" s="9"/>
+      <c r="U18" s="7"/>
     </row>
     <row r="19" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="47"/>
-      <c r="U19" s="48"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2149,16 +2193,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2186,7 +2230,7 @@
         <v>0.81105240000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2200,7 +2244,7 @@
         <v>0.57972380000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2258,7 @@
         <v>0.77683599999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2228,13 +2272,100 @@
         <v>0.223164</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f>C2</f>
+        <v>0.75691330000000001</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" ref="C8">B8*MMULT(D2:E2, $B$10:$B$11)</f>
+        <v>0.47296951766176237</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="59">
+        <v>0.47296951766176237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>B3</f>
+        <v>0.24308669999999999</v>
+      </c>
+      <c r="C9" cm="1">
+        <f t="array" ref="C9">B9*MMULT(D3:E3, $B$10:$B$11)</f>
+        <v>8.6321909559388621E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="59">
+        <v>0.38599311034018136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f>E4</f>
+        <v>0.77683599999999997</v>
+      </c>
+      <c r="C10" cm="1">
+        <f t="array" ref="C10">B10*MMULT(B4:C4, $B$8:$B$9)</f>
+        <v>0.38599311034018136</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="59">
+        <v>8.6321909559388621E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <f>D5</f>
+        <v>0.223164</v>
+      </c>
+      <c r="C11" cm="1">
+        <f t="array" ref="C11">B11*MMULT(B5:C5, $B$8:$B$9)</f>
+        <v>5.4715462438667553E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="59">
+        <v>5.4715462438667553E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E8:F11">
+    <sortCondition descending="1" ref="F8:F11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2260,945 +2391,945 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="56" t="s">
+      <c r="N1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="44" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="E2" s="52" t="s">
+      <c r="C2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="H2" s="52" t="s">
+      <c r="F2" s="58"/>
+      <c r="H2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="K2" s="52" t="s">
+      <c r="I2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="N2" s="52" t="s">
+      <c r="L2" s="58"/>
+      <c r="N2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="Q2" s="52" t="s">
+      <c r="O2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="52"/>
+      <c r="R2" s="58"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="42" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="43">
         <v>0.75691330000000001</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="43">
         <v>0.24308669999999999</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="43">
         <v>0.77683599999999997</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="43">
         <v>0.223164</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="43">
         <v>0.81105240000000001</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="43">
         <v>0.18894759999999999</v>
       </c>
-      <c r="K6" s="51">
+      <c r="K6" s="43">
         <v>0.29058129999999999</v>
       </c>
-      <c r="L6" s="51">
+      <c r="L6" s="43">
         <v>0.70941869999999996</v>
       </c>
-      <c r="N6" s="51">
+      <c r="N6" s="43">
         <v>0.57137990000000005</v>
       </c>
-      <c r="O6" s="51">
+      <c r="O6" s="43">
         <v>0.4286201</v>
       </c>
-      <c r="Q6" s="51">
+      <c r="Q6" s="43">
         <v>0.57972380000000001</v>
       </c>
-      <c r="R6" s="51">
+      <c r="R6" s="43">
         <v>0.42027619999999999</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="41">
         <v>23.1765534</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="41">
         <v>16.541399800000001</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="41">
         <v>29.815231199999999</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="41">
         <v>22.66187</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="41">
         <v>29.622481199999999</v>
       </c>
-      <c r="I7" s="49">
+      <c r="I7" s="41">
         <v>20.798594600000001</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="41">
         <v>18.553594199999999</v>
       </c>
-      <c r="L7" s="49">
+      <c r="L7" s="41">
         <v>23.306821200000002</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="41">
         <v>24.156864800000001</v>
       </c>
-      <c r="O7" s="49">
+      <c r="O7" s="41">
         <v>22.389658600000001</v>
       </c>
-      <c r="Q7" s="49">
+      <c r="Q7" s="41">
         <v>24.000811200000001</v>
       </c>
-      <c r="R7" s="49">
+      <c r="R7" s="41">
         <v>21.858284000000001</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="41">
         <v>10</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="41">
         <v>6</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="41">
         <v>17</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="41">
         <v>12</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="41">
         <v>17</v>
       </c>
-      <c r="I8" s="49">
+      <c r="I8" s="41">
         <v>10</v>
       </c>
-      <c r="K8" s="49">
+      <c r="K8" s="41">
         <v>7</v>
       </c>
-      <c r="L8" s="49">
+      <c r="L8" s="41">
         <v>13</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="41">
         <v>13</v>
       </c>
-      <c r="O8" s="49">
+      <c r="O8" s="41">
         <v>10</v>
       </c>
-      <c r="Q8" s="49">
+      <c r="Q8" s="41">
         <v>13</v>
       </c>
-      <c r="R8" s="49">
+      <c r="R8" s="41">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="41">
         <v>14</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="41">
         <v>8</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="41">
         <v>21</v>
       </c>
-      <c r="F9" s="49">
+      <c r="F9" s="41">
         <v>14</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="41">
         <v>20</v>
       </c>
-      <c r="I9" s="49">
+      <c r="I9" s="41">
         <v>13</v>
       </c>
-      <c r="K9" s="49">
+      <c r="K9" s="41">
         <v>10</v>
       </c>
-      <c r="L9" s="49">
+      <c r="L9" s="41">
         <v>14</v>
       </c>
-      <c r="N9" s="49">
+      <c r="N9" s="41">
         <v>14</v>
       </c>
-      <c r="O9" s="49">
+      <c r="O9" s="41">
         <v>13</v>
       </c>
-      <c r="Q9" s="49">
+      <c r="Q9" s="41">
         <v>14</v>
       </c>
-      <c r="R9" s="49">
+      <c r="R9" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="41">
         <v>17</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="41">
         <v>9</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="41">
         <v>23</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="41">
         <v>16</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="41">
         <v>21</v>
       </c>
-      <c r="I10" s="49">
+      <c r="I10" s="41">
         <v>14</v>
       </c>
-      <c r="K10" s="49">
+      <c r="K10" s="41">
         <v>12</v>
       </c>
-      <c r="L10" s="49">
+      <c r="L10" s="41">
         <v>17</v>
       </c>
-      <c r="N10" s="49">
+      <c r="N10" s="41">
         <v>17</v>
       </c>
-      <c r="O10" s="49">
+      <c r="O10" s="41">
         <v>16</v>
       </c>
-      <c r="Q10" s="49">
+      <c r="Q10" s="41">
         <v>17</v>
       </c>
-      <c r="R10" s="49">
+      <c r="R10" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="41">
         <v>17</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="41">
         <v>10</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="41">
         <v>24</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="41">
         <v>17</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="41">
         <v>24</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="41">
         <v>16</v>
       </c>
-      <c r="K11" s="49">
+      <c r="K11" s="41">
         <v>13</v>
       </c>
-      <c r="L11" s="49">
+      <c r="L11" s="41">
         <v>17</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="41">
         <v>17</v>
       </c>
-      <c r="O11" s="49">
+      <c r="O11" s="41">
         <v>17</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="41">
         <v>17</v>
       </c>
-      <c r="R11" s="49">
+      <c r="R11" s="41">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="41">
         <v>17</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="41">
         <v>12</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="41">
         <v>24</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="41">
         <v>18</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H12" s="41">
         <v>24</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="41">
         <v>17</v>
       </c>
-      <c r="K12" s="49">
+      <c r="K12" s="41">
         <v>13</v>
       </c>
-      <c r="L12" s="49">
+      <c r="L12" s="41">
         <v>20</v>
       </c>
-      <c r="N12" s="49">
+      <c r="N12" s="41">
         <v>20</v>
       </c>
-      <c r="O12" s="49">
+      <c r="O12" s="41">
         <v>17</v>
       </c>
-      <c r="Q12" s="49">
+      <c r="Q12" s="41">
         <v>20</v>
       </c>
-      <c r="R12" s="49">
+      <c r="R12" s="41">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="41">
         <v>20</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="41">
         <v>13</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E13" s="41">
         <v>27</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="41">
         <v>20</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="41">
         <v>27</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I13" s="41">
         <v>17</v>
       </c>
-      <c r="K13" s="49">
+      <c r="K13" s="41">
         <v>16</v>
       </c>
-      <c r="L13" s="49">
+      <c r="L13" s="41">
         <v>21</v>
       </c>
-      <c r="N13" s="49">
+      <c r="N13" s="41">
         <v>20</v>
       </c>
-      <c r="O13" s="49">
+      <c r="O13" s="41">
         <v>19</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="41">
         <v>20</v>
       </c>
-      <c r="R13" s="49">
+      <c r="R13" s="41">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="41">
         <v>20</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="41">
         <v>13</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="41">
         <v>27</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="41">
         <v>20</v>
       </c>
-      <c r="H14" s="49">
+      <c r="H14" s="41">
         <v>27</v>
       </c>
-      <c r="I14" s="49">
+      <c r="I14" s="41">
         <v>18</v>
       </c>
-      <c r="K14" s="49">
+      <c r="K14" s="41">
         <v>16</v>
       </c>
-      <c r="L14" s="49">
+      <c r="L14" s="41">
         <v>21</v>
       </c>
-      <c r="N14" s="49">
+      <c r="N14" s="41">
         <v>21</v>
       </c>
-      <c r="O14" s="49">
+      <c r="O14" s="41">
         <v>20</v>
       </c>
-      <c r="Q14" s="49">
+      <c r="Q14" s="41">
         <v>20</v>
       </c>
-      <c r="R14" s="49">
+      <c r="R14" s="41">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="41">
         <v>21</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="41">
         <v>15</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="41">
         <v>28</v>
       </c>
-      <c r="F15" s="49">
+      <c r="F15" s="41">
         <v>21</v>
       </c>
-      <c r="H15" s="49">
+      <c r="H15" s="41">
         <v>27</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I15" s="41">
         <v>20</v>
       </c>
-      <c r="K15" s="49">
+      <c r="K15" s="41">
         <v>17</v>
       </c>
-      <c r="L15" s="49">
+      <c r="L15" s="41">
         <v>21</v>
       </c>
-      <c r="N15" s="49">
+      <c r="N15" s="41">
         <v>23</v>
       </c>
-      <c r="O15" s="49">
+      <c r="O15" s="41">
         <v>21</v>
       </c>
-      <c r="Q15" s="49">
+      <c r="Q15" s="41">
         <v>23</v>
       </c>
-      <c r="R15" s="49">
+      <c r="R15" s="41">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="41">
         <v>23</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="41">
         <v>16</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E16" s="41">
         <v>31</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="41">
         <v>23</v>
       </c>
-      <c r="H16" s="49">
+      <c r="H16" s="41">
         <v>29</v>
       </c>
-      <c r="I16" s="49">
+      <c r="I16" s="41">
         <v>20</v>
       </c>
-      <c r="K16" s="49">
+      <c r="K16" s="41">
         <v>17</v>
       </c>
-      <c r="L16" s="49">
+      <c r="L16" s="41">
         <v>24</v>
       </c>
-      <c r="N16" s="49">
+      <c r="N16" s="41">
         <v>24</v>
       </c>
-      <c r="O16" s="49">
+      <c r="O16" s="41">
         <v>22</v>
       </c>
-      <c r="Q16" s="49">
+      <c r="Q16" s="41">
         <v>23</v>
       </c>
-      <c r="R16" s="49">
+      <c r="R16" s="41">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="41">
         <v>24</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="41">
         <v>16</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="41">
         <v>31</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="41">
         <v>23</v>
       </c>
-      <c r="H17" s="49">
+      <c r="H17" s="41">
         <v>30</v>
       </c>
-      <c r="I17" s="49">
+      <c r="I17" s="41">
         <v>21</v>
       </c>
-      <c r="K17" s="49">
+      <c r="K17" s="41">
         <v>19</v>
       </c>
-      <c r="L17" s="49">
+      <c r="L17" s="41">
         <v>24</v>
       </c>
-      <c r="N17" s="49">
+      <c r="N17" s="41">
         <v>24</v>
       </c>
-      <c r="O17" s="49">
+      <c r="O17" s="41">
         <v>23</v>
       </c>
-      <c r="Q17" s="49">
+      <c r="Q17" s="41">
         <v>24</v>
       </c>
-      <c r="R17" s="49">
+      <c r="R17" s="41">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="41">
         <v>24</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="41">
         <v>17</v>
       </c>
-      <c r="E18" s="49">
+      <c r="E18" s="41">
         <v>31</v>
       </c>
-      <c r="F18" s="49">
+      <c r="F18" s="41">
         <v>24</v>
       </c>
-      <c r="H18" s="49">
+      <c r="H18" s="41">
         <v>31</v>
       </c>
-      <c r="I18" s="49">
+      <c r="I18" s="41">
         <v>22</v>
       </c>
-      <c r="K18" s="49">
+      <c r="K18" s="41">
         <v>20</v>
       </c>
-      <c r="L18" s="49">
+      <c r="L18" s="41">
         <v>24</v>
       </c>
-      <c r="N18" s="49">
+      <c r="N18" s="41">
         <v>26</v>
       </c>
-      <c r="O18" s="49">
+      <c r="O18" s="41">
         <v>24</v>
       </c>
-      <c r="Q18" s="49">
+      <c r="Q18" s="41">
         <v>26</v>
       </c>
-      <c r="R18" s="49">
+      <c r="R18" s="41">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="41">
         <v>25</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="41">
         <v>19</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="41">
         <v>31</v>
       </c>
-      <c r="F19" s="49">
+      <c r="F19" s="41">
         <v>24</v>
       </c>
-      <c r="H19" s="49">
+      <c r="H19" s="41">
         <v>32</v>
       </c>
-      <c r="I19" s="49">
+      <c r="I19" s="41">
         <v>23</v>
       </c>
-      <c r="K19" s="49">
+      <c r="K19" s="41">
         <v>20</v>
       </c>
-      <c r="L19" s="49">
+      <c r="L19" s="41">
         <v>24</v>
       </c>
-      <c r="N19" s="49">
+      <c r="N19" s="41">
         <v>27</v>
       </c>
-      <c r="O19" s="49">
+      <c r="O19" s="41">
         <v>24</v>
       </c>
-      <c r="Q19" s="49">
+      <c r="Q19" s="41">
         <v>27</v>
       </c>
-      <c r="R19" s="49">
+      <c r="R19" s="41">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="41">
         <v>27</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="41">
         <v>20</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="41">
         <v>34</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="41">
         <v>25</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H20" s="41">
         <v>34</v>
       </c>
-      <c r="I20" s="49">
+      <c r="I20" s="41">
         <v>24</v>
       </c>
-      <c r="K20" s="49">
+      <c r="K20" s="41">
         <v>20</v>
       </c>
-      <c r="L20" s="49">
+      <c r="L20" s="41">
         <v>27</v>
       </c>
-      <c r="N20" s="49">
+      <c r="N20" s="41">
         <v>27</v>
       </c>
-      <c r="O20" s="49">
+      <c r="O20" s="41">
         <v>26</v>
       </c>
-      <c r="Q20" s="49">
+      <c r="Q20" s="41">
         <v>27</v>
       </c>
-      <c r="R20" s="49">
+      <c r="R20" s="41">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="41">
         <v>27</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="41">
         <v>20</v>
       </c>
-      <c r="E21" s="49">
+      <c r="E21" s="41">
         <v>34</v>
       </c>
-      <c r="F21" s="49">
+      <c r="F21" s="41">
         <v>27</v>
       </c>
-      <c r="H21" s="49">
+      <c r="H21" s="41">
         <v>34</v>
       </c>
-      <c r="I21" s="49">
+      <c r="I21" s="41">
         <v>24</v>
       </c>
-      <c r="K21" s="49">
+      <c r="K21" s="41">
         <v>23</v>
       </c>
-      <c r="L21" s="49">
+      <c r="L21" s="41">
         <v>27</v>
       </c>
-      <c r="N21" s="49">
+      <c r="N21" s="41">
         <v>28</v>
       </c>
-      <c r="O21" s="49">
+      <c r="O21" s="41">
         <v>27</v>
       </c>
-      <c r="Q21" s="49">
+      <c r="Q21" s="41">
         <v>27</v>
       </c>
-      <c r="R21" s="49">
+      <c r="R21" s="41">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="41">
         <v>28</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="41">
         <v>21</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E22" s="41">
         <v>34</v>
       </c>
-      <c r="F22" s="49">
+      <c r="F22" s="41">
         <v>27</v>
       </c>
-      <c r="H22" s="49">
+      <c r="H22" s="41">
         <v>34</v>
       </c>
-      <c r="I22" s="49">
+      <c r="I22" s="41">
         <v>25</v>
       </c>
-      <c r="K22" s="49">
+      <c r="K22" s="41">
         <v>23</v>
       </c>
-      <c r="L22" s="49">
+      <c r="L22" s="41">
         <v>28</v>
       </c>
-      <c r="N22" s="49">
+      <c r="N22" s="41">
         <v>30</v>
       </c>
-      <c r="O22" s="49">
+      <c r="O22" s="41">
         <v>27</v>
       </c>
-      <c r="Q22" s="49">
+      <c r="Q22" s="41">
         <v>30</v>
       </c>
-      <c r="R22" s="49">
+      <c r="R22" s="41">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="41">
         <v>30</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="41">
         <v>23</v>
       </c>
-      <c r="E23" s="49">
+      <c r="E23" s="41">
         <v>36</v>
       </c>
-      <c r="F23" s="49">
+      <c r="F23" s="41">
         <v>28</v>
       </c>
-      <c r="H23" s="49">
+      <c r="H23" s="41">
         <v>37</v>
       </c>
-      <c r="I23" s="49">
+      <c r="I23" s="41">
         <v>27</v>
       </c>
-      <c r="K23" s="49">
+      <c r="K23" s="41">
         <v>24</v>
       </c>
-      <c r="L23" s="49">
+      <c r="L23" s="41">
         <v>29</v>
       </c>
-      <c r="N23" s="49">
+      <c r="N23" s="41">
         <v>30</v>
       </c>
-      <c r="O23" s="49">
+      <c r="O23" s="41">
         <v>28</v>
       </c>
-      <c r="Q23" s="49">
+      <c r="Q23" s="41">
         <v>30</v>
       </c>
-      <c r="R23" s="49">
+      <c r="R23" s="41">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="41">
         <v>31</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="41">
         <v>23</v>
       </c>
-      <c r="E24" s="49">
+      <c r="E24" s="41">
         <v>38</v>
       </c>
-      <c r="F24" s="49">
+      <c r="F24" s="41">
         <v>30</v>
       </c>
-      <c r="H24" s="49">
+      <c r="H24" s="41">
         <v>38</v>
       </c>
-      <c r="I24" s="49">
+      <c r="I24" s="41">
         <v>27</v>
       </c>
-      <c r="K24" s="49">
+      <c r="K24" s="41">
         <v>26</v>
       </c>
-      <c r="L24" s="49">
+      <c r="L24" s="41">
         <v>31</v>
       </c>
-      <c r="N24" s="49">
+      <c r="N24" s="41">
         <v>31</v>
       </c>
-      <c r="O24" s="49">
+      <c r="O24" s="41">
         <v>30</v>
       </c>
-      <c r="Q24" s="49">
+      <c r="Q24" s="41">
         <v>31</v>
       </c>
-      <c r="R24" s="49">
+      <c r="R24" s="41">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="49">
+      <c r="B25" s="41">
         <v>32</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25" s="41">
         <v>26</v>
       </c>
-      <c r="E25" s="49">
+      <c r="E25" s="41">
         <v>38</v>
       </c>
-      <c r="F25" s="49">
+      <c r="F25" s="41">
         <v>31</v>
       </c>
-      <c r="H25" s="49">
+      <c r="H25" s="41">
         <v>40</v>
       </c>
-      <c r="I25" s="49">
+      <c r="I25" s="41">
         <v>29</v>
       </c>
-      <c r="K25" s="49">
+      <c r="K25" s="41">
         <v>27</v>
       </c>
-      <c r="L25" s="49">
+      <c r="L25" s="41">
         <v>31</v>
       </c>
-      <c r="N25" s="49">
+      <c r="N25" s="41">
         <v>34</v>
       </c>
-      <c r="O25" s="49">
+      <c r="O25" s="41">
         <v>31</v>
       </c>
-      <c r="Q25" s="49">
+      <c r="Q25" s="41">
         <v>34</v>
       </c>
-      <c r="R25" s="49">
+      <c r="R25" s="41">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B26" s="41">
         <v>34</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="41">
         <v>27</v>
       </c>
-      <c r="E26" s="49">
+      <c r="E26" s="41">
         <v>41</v>
       </c>
-      <c r="F26" s="49">
+      <c r="F26" s="41">
         <v>33</v>
       </c>
-      <c r="H26" s="49">
+      <c r="H26" s="41">
         <v>41</v>
       </c>
-      <c r="I26" s="49">
+      <c r="I26" s="41">
         <v>31</v>
       </c>
-      <c r="K26" s="49">
+      <c r="K26" s="41">
         <v>30</v>
       </c>
-      <c r="L26" s="49">
+      <c r="L26" s="41">
         <v>34</v>
       </c>
-      <c r="N26" s="49">
+      <c r="N26" s="41">
         <v>35</v>
       </c>
-      <c r="O26" s="49">
+      <c r="O26" s="41">
         <v>34</v>
       </c>
-      <c r="Q26" s="49">
+      <c r="Q26" s="41">
         <v>35</v>
       </c>
-      <c r="R26" s="49">
+      <c r="R26" s="41">
         <v>32</v>
       </c>
     </row>

</xml_diff>